<commit_message>
Added documentation for 5th return
</commit_message>
<xml_diff>
--- a/Documentation/Semaine 2/Journal de travail Renaud Grégory TPI.xlsx
+++ b/Documentation/Semaine 2/Journal de travail Renaud Grégory TPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/ph62ldr_eduvaud_ch/Documents/TPI/Semaine 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="752" documentId="13_ncr:1_{0FACF0AD-6438-4E55-9B2C-E5A3B84245AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAFBCC4B-E2D9-40E3-82D5-560A82C611AD}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E93AF827-F335-4273-9BF2-1B7E35411D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7079C538-956F-4B36-B6F8-058FC1A7098D}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{E616EBF9-A1E1-4B05-B307-B39FC77B0801}"/>
   </bookViews>
@@ -1846,10 +1846,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{276EA92B-46E1-49DE-A871-36F19432AE6D}" name="Catégorie" displayName="Catégorie" ref="A1:A42" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:A42" xr:uid="{276EA92B-46E1-49DE-A871-36F19432AE6D}"/>
@@ -2163,8 +2159,8 @@
   <dimension ref="A1:I1196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4165,9 +4161,9 @@
       <c r="I78" s="15"/>
     </row>
     <row r="79" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
       <c r="D79" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4179,9 +4175,9 @@
       <c r="I79" s="15"/>
     </row>
     <row r="80" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
       <c r="D80" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4193,9 +4189,9 @@
       <c r="I80" s="15"/>
     </row>
     <row r="81" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
       <c r="D81" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4207,9 +4203,9 @@
       <c r="I81" s="15"/>
     </row>
     <row r="82" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
       <c r="D82" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4221,9 +4217,9 @@
       <c r="I82" s="15"/>
     </row>
     <row r="83" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
       <c r="D83" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4235,9 +4231,9 @@
       <c r="I83" s="15"/>
     </row>
     <row r="84" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
       <c r="D84" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4249,9 +4245,9 @@
       <c r="I84" s="15"/>
     </row>
     <row r="85" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
       <c r="D85" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4263,9 +4259,9 @@
       <c r="I85" s="15"/>
     </row>
     <row r="86" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
       <c r="D86" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4277,9 +4273,9 @@
       <c r="I86" s="15"/>
     </row>
     <row r="87" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
       <c r="D87" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4291,9 +4287,9 @@
       <c r="I87" s="15"/>
     </row>
     <row r="88" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
       <c r="D88" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4305,9 +4301,9 @@
       <c r="I88" s="15"/>
     </row>
     <row r="89" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
       <c r="D89" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4319,9 +4315,9 @@
       <c r="I89" s="15"/>
     </row>
     <row r="90" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
       <c r="D90" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4333,9 +4329,9 @@
       <c r="I90" s="15"/>
     </row>
     <row r="91" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
+      <c r="A91" s="3"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
       <c r="D91" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4347,9 +4343,9 @@
       <c r="I91" s="15"/>
     </row>
     <row r="92" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
+      <c r="A92" s="3"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
       <c r="D92" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4361,9 +4357,9 @@
       <c r="I92" s="15"/>
     </row>
     <row r="93" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
       <c r="D93" s="4">
         <f t="shared" si="4"/>
         <v>0</v>

</xml_diff>